<commit_message>
Wrong scale for survey SEs, fixed that
</commit_message>
<xml_diff>
--- a/model_alts/ss/base/SS_EBSWP.xlsx
+++ b/model_alts/ss/base/SS_EBSWP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/_mymods/ebswp/model_alts/ss/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A892B436-4057-694E-8850-591BB9185FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B22546-FD68-1E40-9650-C7C664BE0466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{F61E7810-3D62-914B-82A0-DB45FEE13A29}"/>
   </bookViews>
@@ -29671,8 +29671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5745DEC0-F381-7748-8EDF-D212E2A39ED2}">
   <dimension ref="A1:AF368"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A334" zoomScale="74" workbookViewId="0">
-      <selection activeCell="A369" sqref="A1:AN369"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A96" zoomScale="74" workbookViewId="0">
+      <selection activeCell="F100" sqref="F100:F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29767,7 +29767,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
@@ -31387,7 +31387,7 @@
         <v>3640.1060000000002</v>
       </c>
       <c r="E100" s="1">
-        <v>739.84286320000001</v>
+        <v>0.20324761509692299</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -31421,7 +31421,7 @@
         <v>2955.1149999999998</v>
       </c>
       <c r="E102">
-        <v>498.38687169999997</v>
+        <v>0.16865227637503108</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -31438,7 +31438,7 @@
         <v>3590.6950000000002</v>
       </c>
       <c r="E103" s="1">
-        <v>574.52355799999998</v>
+        <v>0.16000344167354785</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -31472,7 +31472,7 @@
         <v>4202.143</v>
       </c>
       <c r="E105">
-        <v>999.45010360000003</v>
+        <v>0.23784295384521661</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -31489,7 +31489,7 @@
         <v>3613.94</v>
       </c>
       <c r="E106" s="1">
-        <v>500.1019139</v>
+        <v>0.13838135494778553</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -31523,7 +31523,7 @@
         <v>4330.0079999999998</v>
       </c>
       <c r="E108" s="1">
-        <v>580.46761230000004</v>
+        <v>0.13405693760842938</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -31557,7 +31557,7 @@
         <v>4016.18</v>
       </c>
       <c r="E110" s="1">
-        <v>642.60262239999997</v>
+        <v>0.16000344167841082</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -31591,7 +31591,7 @@
         <v>1887.421</v>
       </c>
       <c r="E112" s="1">
-        <v>318.31784809999999</v>
+        <v>0.16865227636017613</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -31608,7 +31608,7 @@
         <v>2288.0700000000002</v>
       </c>
       <c r="E113" s="1">
-        <v>445.25563149999999</v>
+        <v>0.19459878041318665</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -31625,7 +31625,7 @@
         <v>1407.479</v>
       </c>
       <c r="E114" s="1">
-        <v>464.94475169999998</v>
+        <v>0.33033867766410724</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -31642,7 +31642,7 @@
         <v>1323.06</v>
       </c>
       <c r="E115">
-        <v>503.4887976</v>
+        <v>0.38054872613486918</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -31659,7 +31659,7 @@
         <v>2651.1759999999999</v>
       </c>
       <c r="E116" s="1">
-        <v>687.88748840000005</v>
+        <v>0.2594650405706751</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -31693,7 +31693,7 @@
         <v>2298.9409999999998</v>
       </c>
       <c r="E118" s="1">
-        <v>417.54637389999999</v>
+        <v>0.18162552840634014</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -31727,7 +31727,7 @@
         <v>4726.5990000000002</v>
       </c>
       <c r="E120" s="1">
-        <v>949.05300109999996</v>
+        <v>0.20078982818301275</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -31761,7 +31761,7 @@
         <v>4828.8896869999999</v>
       </c>
       <c r="E122" s="1">
-        <v>438.52482040000001</v>
+        <v>9.0812764180669928E-2</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -31795,7 +31795,7 @@
         <v>2499.4010640000001</v>
       </c>
       <c r="E124">
-        <v>477.33650729999999</v>
+        <v>0.19098035692442195</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -31812,7 +31812,7 @@
         <v>3820.9554149999999</v>
       </c>
       <c r="E125">
-        <v>327.58364080000001</v>
+        <v>8.5733437117323716E-2</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -31829,7 +31829,7 @@
         <v>8980.6900929999993</v>
       </c>
       <c r="E126">
-        <v>761.8922609</v>
+        <v>8.4836716667670897E-2</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -31846,7 +31846,7 @@
         <v>6472.5730359999998</v>
       </c>
       <c r="E127">
-        <v>704.21149390000005</v>
+        <v>0.10879931211022646</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -31863,7 +31863,7 @@
         <v>7558.5239149999998</v>
       </c>
       <c r="E128">
-        <v>749.09249829999999</v>
+        <v>9.9105659613435246E-2</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -31880,7 +31880,7 @@
         <v>7157.5728589999999</v>
       </c>
       <c r="E129">
-        <v>641.11998189999997</v>
+        <v>8.9572260671276244E-2</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -31897,7 +31897,7 @@
         <v>7833.2076619999998</v>
       </c>
       <c r="E130">
-        <v>716.91674660000001</v>
+        <v>9.1522755113191329E-2</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -31914,7 +31914,7 @@
         <v>11680.45377</v>
       </c>
       <c r="E131">
-        <v>1137.238564</v>
+        <v>9.7362532859885637E-2</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -31931,7 +31931,7 @@
         <v>9975.7765130000007</v>
       </c>
       <c r="E132">
-        <v>832.12143719999995</v>
+        <v>8.3414202003785395E-2</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -31948,7 +31948,7 @@
         <v>11408.407670000001</v>
       </c>
       <c r="E133">
-        <v>1380.242802</v>
+        <v>0.12098470197813328</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -31965,7 +31965,7 @@
         <v>7235.1690429999999</v>
       </c>
       <c r="E134">
-        <v>608.80438200000003</v>
+        <v>8.4145149668481634E-2</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -31982,7 +31982,7 @@
         <v>6643.1053659999998</v>
       </c>
       <c r="E135">
-        <v>601.05397379999999</v>
+        <v>9.0477862488264504E-2</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -31999,7 +31999,7 @@
         <v>7822.5581110000003</v>
       </c>
       <c r="E136">
-        <v>630.44894099999999</v>
+        <v>8.0593705032816459E-2</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -32016,7 +32016,7 @@
         <v>6886.6390430000001</v>
       </c>
       <c r="E137">
-        <v>682.93648129999997</v>
+        <v>9.9168328270984124E-2</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -32033,7 +32033,7 @@
         <v>6554.9205259999999</v>
       </c>
       <c r="E138">
-        <v>790.67881439999996</v>
+        <v>0.12062370722326587</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -32050,7 +32050,7 @@
         <v>3990.5807709999999</v>
       </c>
       <c r="E139">
-        <v>335.75338640000001</v>
+        <v>8.4136471773722188E-2</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -32067,7 +32067,7 @@
         <v>4458.6464230000001</v>
       </c>
       <c r="E140">
-        <v>383.43037880000003</v>
+        <v>8.5997036414923636E-2</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -32084,7 +32084,7 @@
         <v>3454.7122239999999</v>
       </c>
       <c r="E141">
-        <v>269.6325784</v>
+        <v>7.8047768067873668E-2</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -32101,7 +32101,7 @@
         <v>5592.7946250000005</v>
       </c>
       <c r="E142">
-        <v>492.36046470000002</v>
+        <v>8.8034783630196317E-2</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -32118,7 +32118,7 @@
         <v>7052.5389489999998</v>
       </c>
       <c r="E143">
-        <v>760.01306790000001</v>
+        <v>0.10776446232994778</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -32135,7 +32135,7 @@
         <v>6014.1346759999997</v>
       </c>
       <c r="E144">
-        <v>484.33776899999998</v>
+        <v>8.0533242950610637E-2</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -32152,7 +32152,7 @@
         <v>6720.6883500000004</v>
       </c>
       <c r="E145">
-        <v>528.53339370000003</v>
+        <v>7.8642747018614539E-2</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -32169,7 +32169,7 @@
         <v>11175.832539999999</v>
       </c>
       <c r="E146">
-        <v>1016.651414</v>
+        <v>9.0968740839776407E-2</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -32186,7 +32186,7 @@
         <v>5632.534028</v>
       </c>
       <c r="E147">
-        <v>449.98631669999997</v>
+        <v>7.989056337042337E-2</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -32203,7 +32203,7 @@
         <v>6882.763183</v>
       </c>
       <c r="E148">
-        <v>623.16305609999995</v>
+        <v>9.0539662564473267E-2</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -32220,7 +32220,7 @@
         <v>4113.0996459999997</v>
       </c>
       <c r="E149">
-        <v>395.27263010000001</v>
+        <v>9.6100912722696538E-2</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -32237,7 +32237,7 @@
         <v>6867.444708</v>
       </c>
       <c r="E150">
-        <v>792.7079238</v>
+        <v>0.11542982251849242</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -32254,7 +32254,7 @@
         <v>4275.9849530000001</v>
       </c>
       <c r="E151">
-        <v>479.4599217</v>
+        <v>0.11212853341862543</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -32271,7 +32271,7 @@
         <v>2851.9643160000001</v>
       </c>
       <c r="E152">
-        <v>430.59137290000001</v>
+        <v>0.15098063130885261</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -32288,7 +32288,7 @@
         <v>5174.0234959999998</v>
       </c>
       <c r="E153">
-        <v>584.5527161</v>
+        <v>0.11297836520300178</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -32305,7 +32305,7 @@
         <v>4540.9727190000003</v>
       </c>
       <c r="E154">
-        <v>358.18678469999998</v>
+        <v>7.8878867340757511E-2</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -32322,7 +32322,7 @@
         <v>5173.0013550000003</v>
       </c>
       <c r="E155">
-        <v>401.80583460000003</v>
+        <v>7.7673637995789774E-2</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -32339,7 +32339,7 @@
         <v>6658.3685260000002</v>
       </c>
       <c r="E156">
-        <v>539.28183590000003</v>
+        <v>8.0993089192071557E-2</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -32356,7 +32356,7 @@
         <v>11692.74865</v>
       </c>
       <c r="E157">
-        <v>825.81606799999997</v>
+        <v>7.0626342250160318E-2</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -32373,7 +32373,7 @@
         <v>10654.0134</v>
       </c>
       <c r="E158">
-        <v>702.956098</v>
+        <v>6.5980403028214701E-2</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -32390,7 +32390,7 @@
         <v>8427.3674599999995</v>
       </c>
       <c r="E159">
-        <v>779.27359980000006</v>
+        <v>9.2469398480459764E-2</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -32407,7 +32407,7 @@
         <v>8914.5438730000005</v>
       </c>
       <c r="E160">
-        <v>588.78606060000004</v>
+        <v>6.6047805584679514E-2</v>
       </c>
     </row>
     <row r="161" spans="1:27" x14ac:dyDescent="0.2">
@@ -32424,7 +32424,7 @@
         <v>4039.3067540000002</v>
       </c>
       <c r="E161">
-        <v>447.61320669999998</v>
+        <v>0.11081436344410894</v>
       </c>
     </row>
     <row r="162" spans="1:27" x14ac:dyDescent="0.2">
@@ -32441,7 +32441,7 @@
         <v>9443.6685080000007</v>
       </c>
       <c r="E162">
-        <v>629.43035499999996</v>
+        <v>6.6651042914815523E-2</v>
       </c>
     </row>
     <row r="163" spans="1:27" x14ac:dyDescent="0.2">
@@ -32475,7 +32475,7 @@
         <v>4807.9667460000001</v>
       </c>
       <c r="E164">
-        <v>342.84146199999998</v>
+        <v>7.1306953669184131E-2</v>
       </c>
     </row>
     <row r="165" spans="1:27" x14ac:dyDescent="0.2">
@@ -32492,7 +32492,7 @@
         <v>6508.7325179999998</v>
       </c>
       <c r="E165">
-        <v>505.29923509999998</v>
+        <v>7.7634045292626047E-2</v>
       </c>
     </row>
     <row r="166" spans="1:27" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Thanks to Ian Taylor for help fixing zero variance (and for me not using an old hash for installing r4ss
</commit_message>
<xml_diff>
--- a/model_alts/ss/base/SS_EBSWP.xlsx
+++ b/model_alts/ss/base/SS_EBSWP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jim/_mymods/ebswp/model_alts/ss/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B22546-FD68-1E40-9650-C7C664BE0466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0D7B33-0AF4-8846-8130-57D0B4A1BD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{F61E7810-3D62-914B-82A0-DB45FEE13A29}"/>
   </bookViews>
@@ -4103,8 +4103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001B5695-A6DF-A940-8036-AAA346CF2023}">
   <dimension ref="A1:AB382"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:T7"/>
+    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="N21" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4291,6 +4291,54 @@
       <c r="F7">
         <v>-2</v>
       </c>
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K7">
+        <v>0.14449999999999999</v>
+      </c>
+      <c r="L7">
+        <v>0.32050000000000001</v>
+      </c>
+      <c r="M7">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="N7">
+        <v>0.45050000000000001</v>
+      </c>
+      <c r="O7">
+        <v>0.47349999999999998</v>
+      </c>
+      <c r="P7">
+        <v>0.48149999999999998</v>
+      </c>
+      <c r="Q7">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="R7">
+        <v>0.5</v>
+      </c>
+      <c r="S7">
+        <v>0.5</v>
+      </c>
+      <c r="T7">
+        <v>0.5</v>
+      </c>
+      <c r="U7">
+        <v>0.5</v>
+      </c>
+      <c r="V7">
+        <v>0.5</v>
+      </c>
+      <c r="W7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -4439,49 +4487,49 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K10">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L10">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M10">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N10">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O10">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P10">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q10">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R10">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S10">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T10">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U10">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V10">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W10">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
@@ -4508,49 +4556,49 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K11">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L11">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M11">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N11">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O11">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P11">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q11">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R11">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S11">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T11">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U11">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V11">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W11">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
@@ -4577,49 +4625,49 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K12">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L12">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M12">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N12">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O12">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P12">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q12">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R12">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S12">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T12">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U12">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V12">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W12">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
@@ -4646,49 +4694,49 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K13">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L13">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M13">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N13">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O13">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P13">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q13">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R13">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S13">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T13">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U13">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V13">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W13">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
@@ -4715,49 +4763,49 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K14">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L14">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M14">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N14">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O14">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P14">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q14">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R14">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S14">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T14">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U14">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V14">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W14">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
@@ -4784,49 +4832,49 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K15">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L15">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M15">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N15">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O15">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P15">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q15">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R15">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S15">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T15">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U15">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V15">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W15">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
@@ -4853,49 +4901,49 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K16">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L16">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M16">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N16">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O16">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P16">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q16">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R16">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S16">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T16">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U16">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V16">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W16">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.2">
@@ -4922,49 +4970,49 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K17">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L17">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M17">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N17">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O17">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P17">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q17">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R17">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S17">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T17">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U17">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V17">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W17">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.2">
@@ -4991,49 +5039,49 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K18">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L18">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M18">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N18">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O18">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P18">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q18">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R18">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S18">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T18">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U18">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V18">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W18">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.2">
@@ -5060,49 +5108,49 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K19">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L19">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M19">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N19">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O19">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P19">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q19">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R19">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S19">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T19">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U19">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V19">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W19">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.2">
@@ -5129,49 +5177,49 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K20">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L20">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M20">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N20">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O20">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P20">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q20">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R20">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S20">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T20">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U20">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V20">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W20">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.2">
@@ -5198,49 +5246,49 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K21">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L21">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M21">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N21">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O21">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P21">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q21">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R21">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S21">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T21">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U21">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V21">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W21">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.2">
@@ -5266,49 +5314,49 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K22">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L22">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M22">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N22">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O22">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P22">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q22">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R22">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S22">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T22">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U22">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V22">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W22">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.2">
@@ -5334,49 +5382,49 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K23">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L23">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M23">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N23">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O23">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P23">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q23">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R23">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S23">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T23">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U23">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V23">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W23">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.2">
@@ -5402,49 +5450,49 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K24">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L24">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M24">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N24">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O24">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P24">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q24">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R24">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S24">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T24">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U24">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V24">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W24">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.2">
@@ -5470,49 +5518,49 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K25">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L25">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M25">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N25">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O25">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P25">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q25">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R25">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S25">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T25">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U25">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V25">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W25">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.2">
@@ -5538,49 +5586,49 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K26">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L26">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M26">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N26">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O26">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P26">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q26">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R26">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S26">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T26">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U26">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V26">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W26">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.2">
@@ -5606,49 +5654,49 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J27">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K27">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L27">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M27">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N27">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O27">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P27">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q27">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R27">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S27">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T27">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U27">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V27">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W27">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.2">
@@ -5674,49 +5722,49 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K28">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L28">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M28">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N28">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O28">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P28">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q28">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R28">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S28">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T28">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U28">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V28">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W28">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.2">
@@ -5742,49 +5790,49 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K29">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L29">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M29">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N29">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O29">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P29">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q29">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R29">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S29">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T29">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U29">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V29">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W29">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.2">
@@ -5810,49 +5858,49 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J30">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K30">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L30">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M30">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N30">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O30">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P30">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q30">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R30">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S30">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T30">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U30">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V30">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W30">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.2">
@@ -5878,49 +5926,49 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K31">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L31">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M31">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N31">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O31">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P31">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q31">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R31">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S31">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T31">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U31">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V31">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W31">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.2">
@@ -5946,49 +5994,49 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K32">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L32">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M32">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N32">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O32">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P32">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q32">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R32">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S32">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T32">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U32">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V32">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W32">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.2">
@@ -6014,49 +6062,49 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K33">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L33">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M33">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N33">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O33">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P33">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q33">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R33">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S33">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T33">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U33">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V33">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W33">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.2">
@@ -6082,49 +6130,49 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K34">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L34">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M34">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N34">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O34">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P34">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q34">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R34">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S34">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T34">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U34">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V34">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W34">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.2">
@@ -6150,49 +6198,49 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J35">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K35">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L35">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M35">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N35">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O35">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P35">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q35">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R35">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S35">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T35">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U35">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V35">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W35">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.2">
@@ -6218,49 +6266,49 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J36">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K36">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L36">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M36">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N36">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O36">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P36">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q36">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R36">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S36">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T36">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U36">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V36">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W36">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.2">
@@ -6286,49 +6334,49 @@
         <v>0</v>
       </c>
       <c r="I37">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J37">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K37">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L37">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M37">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N37">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O37">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P37">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q37">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R37">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S37">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T37">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U37">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V37">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W37">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.2">
@@ -6354,49 +6402,49 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J38">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K38">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L38">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M38">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N38">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O38">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P38">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q38">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R38">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S38">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T38">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U38">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V38">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W38">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.2">
@@ -6422,49 +6470,49 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K39">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L39">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M39">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N39">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O39">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P39">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q39">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R39">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S39">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T39">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U39">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V39">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W39">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.2">
@@ -6490,49 +6538,49 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K40">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L40">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M40">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N40">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O40">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P40">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q40">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R40">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S40">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T40">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U40">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V40">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W40">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.2">
@@ -6558,49 +6606,49 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J41">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K41">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L41">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M41">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N41">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O41">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P41">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q41">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R41">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S41">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T41">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U41">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V41">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W41">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.2">
@@ -6626,49 +6674,49 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J42">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K42">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L42">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M42">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N42">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O42">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P42">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q42">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R42">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S42">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T42">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U42">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V42">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W42">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.2">
@@ -6694,49 +6742,49 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J43">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K43">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L43">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M43">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N43">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O43">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P43">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q43">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R43">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S43">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T43">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U43">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V43">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W43">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.2">
@@ -6762,49 +6810,49 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J44">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K44">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L44">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M44">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N44">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O44">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P44">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q44">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R44">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S44">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T44">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U44">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V44">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W44">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.2">
@@ -6830,49 +6878,49 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J45">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K45">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L45">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M45">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N45">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O45">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P45">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q45">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R45">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S45">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T45">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U45">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V45">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W45">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.2">
@@ -6898,49 +6946,49 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J46">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K46">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L46">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M46">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N46">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O46">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P46">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q46">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R46">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S46">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T46">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U46">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V46">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W46">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.2">
@@ -6966,49 +7014,49 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J47">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K47">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L47">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M47">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N47">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O47">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P47">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q47">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R47">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S47">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T47">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U47">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V47">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W47">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.2">
@@ -7034,49 +7082,49 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J48">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K48">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L48">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M48">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N48">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O48">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P48">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q48">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R48">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S48">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T48">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U48">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V48">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W48">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.2">
@@ -7102,49 +7150,49 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J49">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K49">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L49">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M49">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N49">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O49">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P49">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q49">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R49">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S49">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T49">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U49">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V49">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W49">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.2">
@@ -7170,49 +7218,49 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J50">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K50">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L50">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M50">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N50">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O50">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P50">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q50">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R50">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S50">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T50">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U50">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V50">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W50">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.2">
@@ -7238,49 +7286,49 @@
         <v>0</v>
       </c>
       <c r="I51">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J51">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K51">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L51">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M51">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N51">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O51">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P51">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q51">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R51">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S51">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T51">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U51">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V51">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W51">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.2">
@@ -7306,49 +7354,49 @@
         <v>0</v>
       </c>
       <c r="I52">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J52">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K52">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L52">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M52">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N52">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O52">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P52">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q52">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R52">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S52">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T52">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U52">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V52">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W52">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.2">
@@ -7374,49 +7422,49 @@
         <v>0</v>
       </c>
       <c r="I53">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J53">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K53">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L53">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M53">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N53">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O53">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P53">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q53">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R53">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S53">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T53">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U53">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V53">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W53">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.2">
@@ -7442,49 +7490,49 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J54">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K54">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L54">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M54">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N54">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O54">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P54">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q54">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R54">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S54">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T54">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U54">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V54">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W54">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.2">
@@ -7510,49 +7558,49 @@
         <v>0</v>
       </c>
       <c r="I55">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J55">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K55">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L55">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M55">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N55">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O55">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P55">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q55">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R55">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S55">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T55">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U55">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V55">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W55">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.2">
@@ -7578,49 +7626,49 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J56">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K56">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L56">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M56">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N56">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O56">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P56">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q56">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R56">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S56">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T56">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U56">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V56">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W56">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.2">
@@ -7646,49 +7694,49 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J57">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K57">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L57">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M57">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N57">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O57">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P57">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q57">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R57">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S57">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T57">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U57">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V57">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W57">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.2">
@@ -7714,49 +7762,49 @@
         <v>0</v>
       </c>
       <c r="I58">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J58">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K58">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L58">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M58">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N58">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O58">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P58">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q58">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R58">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S58">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T58">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U58">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V58">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W58">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.2">
@@ -7782,49 +7830,49 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J59">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K59">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L59">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M59">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N59">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O59">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P59">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q59">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R59">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S59">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T59">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U59">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V59">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W59">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.2">
@@ -7850,49 +7898,49 @@
         <v>0</v>
       </c>
       <c r="I60">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J60">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K60">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L60">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M60">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N60">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O60">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P60">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q60">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R60">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S60">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T60">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U60">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V60">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W60">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.2">
@@ -7918,49 +7966,49 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J61">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K61">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L61">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M61">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N61">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O61">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P61">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q61">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R61">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S61">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T61">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U61">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V61">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W61">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.2">
@@ -7986,49 +8034,49 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J62">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K62">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L62">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M62">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N62">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O62">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P62">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q62">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R62">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S62">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T62">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U62">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V62">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W62">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.2">
@@ -8054,49 +8102,49 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J63">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K63">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L63">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M63">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N63">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O63">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P63">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q63">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R63">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S63">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T63">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U63">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V63">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W63">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.2">
@@ -8122,49 +8170,49 @@
         <v>0</v>
       </c>
       <c r="I64">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J64">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K64">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L64">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M64">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N64">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O64">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P64">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q64">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R64">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S64">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T64">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U64">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V64">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W64">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.2">
@@ -8190,49 +8238,49 @@
         <v>0</v>
       </c>
       <c r="I65">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J65">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K65">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L65">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M65">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N65">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O65">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P65">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q65">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R65">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S65">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T65">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U65">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V65">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W65">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.2">
@@ -8259,49 +8307,49 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J66">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K66">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L66">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M66">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N66">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O66">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P66">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q66">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R66">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S66">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T66">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U66">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V66">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W66">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.2">
@@ -8328,49 +8376,49 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J67">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K67">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L67">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M67">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N67">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O67">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P67">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q67">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R67">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S67">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T67">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U67">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V67">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W67">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.2">
@@ -8397,49 +8445,49 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J68">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K68">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L68">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M68">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N68">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O68">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P68">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q68">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R68">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S68">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T68">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U68">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V68">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W68">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.2">
@@ -8466,49 +8514,49 @@
         <v>0</v>
       </c>
       <c r="I69">
-        <v>8.4881665999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="J69">
-        <v>0.195868126</v>
+        <v>7.8347250400000006E-4</v>
       </c>
       <c r="K69">
-        <v>0.31376278800000001</v>
+        <v>4.5338722865999999E-2</v>
       </c>
       <c r="L69">
-        <v>0.459295544</v>
+        <v>0.14720422185199999</v>
       </c>
       <c r="M69">
-        <v>0.58862360199999997</v>
+        <v>0.24781053644199999</v>
       </c>
       <c r="N69">
-        <v>0.69781833100000001</v>
+        <v>0.31436715811550003</v>
       </c>
       <c r="O69">
-        <v>0.79679873899999998</v>
+        <v>0.37728420291649994</v>
       </c>
       <c r="P69">
-        <v>0.91486126300000004</v>
+        <v>0.44050569813450002</v>
       </c>
       <c r="Q69">
-        <v>1.0569570109999999</v>
+        <v>0.51262415033499997</v>
       </c>
       <c r="R69">
-        <v>1.147231476</v>
+        <v>0.57361573799999999</v>
       </c>
       <c r="S69">
-        <v>1.290106451</v>
+        <v>0.64505322549999999</v>
       </c>
       <c r="T69">
-        <v>1.3879178889999999</v>
+        <v>0.69395894449999995</v>
       </c>
       <c r="U69">
-        <v>1.4316667599999999</v>
+        <v>0.71583337999999996</v>
       </c>
       <c r="V69">
-        <v>1.4070027190000001</v>
+        <v>0.70350135950000003</v>
       </c>
       <c r="W69">
-        <v>1.522866931</v>
+        <v>0.76143346550000002</v>
       </c>
     </row>
     <row r="70" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -29671,8 +29719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5745DEC0-F381-7748-8EDF-D212E2A39ED2}">
   <dimension ref="A1:AF368"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A96" zoomScale="74" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100:F165"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29:G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30191,7 +30239,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>1065</v>
+        <v>1965</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -54000,8 +54048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E93FA1-6279-E047-92E5-CD1E42BC433A}">
   <dimension ref="A1:BG440"/>
   <sheetViews>
-    <sheetView topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="B191" sqref="B191:S191"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80:P80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>